<commit_message>
Many changes in preparation for making this much simpler to re-run each year. Added a python venv with Scrapy and its dependencies; reworked the TODO list to put parts that will be repeated each year into the README; Began to update step 3 to incorporate the previous year's final player attributes file; re-organized the process inputs and outputs with additional subfolders to clarify which inputs/outputs belong to which steps; changed naming conventions on my player attributes file while it is still a WIP; etc.
</commit_message>
<xml_diff>
--- a/docs/06 - FORMULA for Translating Combines to Ratings.xlsx
+++ b/docs/06 - FORMULA for Translating Combines to Ratings.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="137">
   <si>
     <t>SPEED</t>
   </si>
@@ -366,9 +366,6 @@
     <t>If the numbers end up so unbalanced that one is 100+ , check the list below for expected total ACC + AGI and distribute as I see fit.</t>
   </si>
   <si>
-    <t>TOTAL Shuttle + 3-Cone</t>
-  </si>
-  <si>
     <t>TOTAL Acc + Agi</t>
   </si>
   <si>
@@ -406,6 +403,33 @@
   </si>
   <si>
     <t>11.83</t>
+  </si>
+  <si>
+    <t>11.40</t>
+  </si>
+  <si>
+    <t>11.20</t>
+  </si>
+  <si>
+    <t>11.00</t>
+  </si>
+  <si>
+    <t>10.80</t>
+  </si>
+  <si>
+    <t>10.60</t>
+  </si>
+  <si>
+    <t>10.40</t>
+  </si>
+  <si>
+    <t>TOTAL Shutl + 3-Cone Range</t>
+  </si>
+  <si>
+    <t>30.5 - 30.9</t>
+  </si>
+  <si>
+    <t>30.0 - 30.4</t>
   </si>
 </sst>
 </file>
@@ -473,14 +497,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,22 +786,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="9.06640625" style="2"/>
+    <col min="1" max="2" width="9" style="2"/>
     <col min="3" max="3" width="3.59765625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="10.59765625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="9.06640625" style="2"/>
+    <col min="4" max="5" width="11.59765625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9" style="2"/>
     <col min="8" max="8" width="3.59765625" style="2" customWidth="1"/>
-    <col min="9" max="10" width="9.06640625" style="2"/>
+    <col min="9" max="10" width="9" style="2"/>
     <col min="11" max="11" width="3.59765625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.06640625" style="2"/>
+    <col min="12" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
@@ -846,18 +872,18 @@
         <v>50</v>
       </c>
       <c r="D3" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.21</v>
       </c>
       <c r="E3" s="2">
-        <v>6.96</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2">
         <f>ROUND((-86.14428*(D3-(0.5*E3))+148.54528),0)</f>
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="G3" s="2">
         <f>ROUND((-65.78539*(E3-(0.9*D3))+298.87444),0)</f>
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="I3" s="2">
         <v>4</v>
@@ -895,12 +921,12 @@
       <c r="B5" s="2">
         <v>52</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
       <c r="I5" s="2">
         <v>6</v>
       </c>
@@ -919,10 +945,10 @@
       <c r="B6" s="2">
         <v>53</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
       <c r="I6" s="2">
         <v>7</v>
       </c>
@@ -941,10 +967,10 @@
       <c r="B7" s="2">
         <v>54</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
       <c r="I7" s="2">
         <v>8</v>
       </c>
@@ -963,12 +989,12 @@
       <c r="B8" s="2">
         <v>55</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
       <c r="I8" s="2">
         <v>9</v>
       </c>
@@ -987,10 +1013,10 @@
       <c r="B9" s="2">
         <v>56</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
       <c r="I9" s="2">
         <v>10</v>
       </c>
@@ -1009,10 +1035,10 @@
       <c r="B10" s="2">
         <v>57</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
       <c r="I10" s="2">
         <v>11</v>
       </c>
@@ -1031,10 +1057,10 @@
       <c r="B11" s="2">
         <v>58</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
       <c r="I11" s="2">
         <v>12</v>
       </c>
@@ -1072,11 +1098,11 @@
         <v>60</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G13" s="8"/>
       <c r="I13" s="2">
@@ -1097,14 +1123,16 @@
       <c r="B14" s="2">
         <v>61</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="D14" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7">
+        <v>160</v>
+      </c>
       <c r="I14" s="2">
         <v>15</v>
       </c>
@@ -1123,21 +1151,25 @@
       <c r="B15" s="2">
         <v>62</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="D15" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7">
+        <v>161</v>
+      </c>
       <c r="I15" s="2">
         <v>16</v>
       </c>
       <c r="J15" s="2">
         <v>66</v>
       </c>
-      <c r="L15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="M15" s="2">
         <v>62</v>
       </c>
@@ -1149,21 +1181,25 @@
       <c r="B16" s="2">
         <v>63</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="D16" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7">
+        <v>162</v>
+      </c>
       <c r="I16" s="2">
         <v>17</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="5"/>
+      <c r="L16" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="M16" s="2">
         <v>63</v>
       </c>
@@ -1175,14 +1211,16 @@
       <c r="B17" s="2">
         <v>64</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="D17" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7">
+        <v>163</v>
+      </c>
       <c r="I17" s="2">
         <v>18</v>
       </c>
@@ -1190,7 +1228,7 @@
         <v>69</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M17" s="2">
         <v>64</v>
@@ -1203,14 +1241,16 @@
       <c r="B18" s="2">
         <v>65</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="D18" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7">
+        <v>164</v>
+      </c>
       <c r="I18" s="2">
         <v>19</v>
       </c>
@@ -1218,7 +1258,7 @@
         <v>16</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M18" s="2">
         <v>65</v>
@@ -1231,14 +1271,16 @@
       <c r="B19" s="2">
         <v>66</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="D19" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7">
+        <v>165</v>
+      </c>
       <c r="I19" s="2">
         <v>20</v>
       </c>
@@ -1246,7 +1288,7 @@
         <v>72</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M19" s="2">
         <v>66</v>
@@ -1259,14 +1301,16 @@
       <c r="B20" s="2">
         <v>67</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="7">
         <v>11.56</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <v>11.59</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7">
+        <v>166</v>
+      </c>
       <c r="I20" s="2">
         <v>21</v>
       </c>
@@ -1274,7 +1318,7 @@
         <v>73</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M20" s="2">
         <v>67</v>
@@ -1287,14 +1331,16 @@
       <c r="B21" s="2">
         <v>68</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="7">
         <v>11.52</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>11.55</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7">
+        <v>167</v>
+      </c>
       <c r="I21" s="2">
         <v>22</v>
       </c>
@@ -1302,7 +1348,7 @@
         <v>74</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M21" s="2">
         <v>68</v>
@@ -1315,14 +1361,14 @@
       <c r="B22" s="2">
         <v>69</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="7">
         <v>11.48</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="7">
         <v>11.51</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9">
+      <c r="F22" s="7"/>
+      <c r="G22" s="7">
         <v>168</v>
       </c>
       <c r="I22" s="2">
@@ -1332,7 +1378,7 @@
         <v>17</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M22" s="2">
         <v>69</v>
@@ -1345,14 +1391,14 @@
       <c r="B23" s="2">
         <v>70</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="7">
         <v>11.44</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>11.47</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9">
+      <c r="F23" s="7"/>
+      <c r="G23" s="7">
         <v>169</v>
       </c>
       <c r="I23" s="2">
@@ -1362,7 +1408,7 @@
         <v>77</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M23" s="2">
         <v>70</v>
@@ -1375,10 +1421,14 @@
       <c r="B24" s="2">
         <v>71</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9">
+      <c r="D24" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="7">
+        <v>11.43</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7">
         <v>170</v>
       </c>
       <c r="I24" s="2">
@@ -1388,7 +1438,7 @@
         <v>78</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M24" s="2">
         <v>71</v>
@@ -1401,10 +1451,14 @@
       <c r="B25" s="2">
         <v>72</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9">
+      <c r="D25" s="7">
+        <v>11.36</v>
+      </c>
+      <c r="E25" s="7">
+        <v>11.39</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7">
         <v>171</v>
       </c>
       <c r="I25" s="2">
@@ -1414,7 +1468,7 @@
         <v>79</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M25" s="2">
         <v>72</v>
@@ -1427,10 +1481,14 @@
       <c r="B26" s="2">
         <v>73</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9">
+      <c r="D26" s="7">
+        <v>11.32</v>
+      </c>
+      <c r="E26" s="7">
+        <v>11.35</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7">
         <v>172</v>
       </c>
       <c r="I26" s="2">
@@ -1440,7 +1498,7 @@
         <v>18</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M26" s="2">
         <v>73</v>
@@ -1453,10 +1511,14 @@
       <c r="B27" s="2">
         <v>74</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9">
+      <c r="D27" s="7">
+        <v>11.28</v>
+      </c>
+      <c r="E27" s="7">
+        <v>11.31</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7">
         <v>173</v>
       </c>
       <c r="I27" s="2">
@@ -1466,7 +1528,7 @@
         <v>82</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M27" s="2">
         <v>74</v>
@@ -1479,10 +1541,14 @@
       <c r="B28" s="2">
         <v>75</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9">
+      <c r="D28" s="7">
+        <v>11.24</v>
+      </c>
+      <c r="E28" s="7">
+        <v>11.27</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7">
         <v>174</v>
       </c>
       <c r="I28" s="2">
@@ -1492,7 +1558,7 @@
         <v>83</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M28" s="2">
         <v>75</v>
@@ -1505,10 +1571,14 @@
       <c r="B29" s="2">
         <v>76</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9">
+      <c r="D29" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="7">
+        <v>11.23</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7">
         <v>175</v>
       </c>
       <c r="I29" s="2">
@@ -1518,7 +1588,7 @@
         <v>84</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="M29" s="2">
         <v>76</v>
@@ -1531,10 +1601,14 @@
       <c r="B30" s="2">
         <v>77</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9">
+      <c r="D30" s="7">
+        <v>11.16</v>
+      </c>
+      <c r="E30" s="7">
+        <v>11.19</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7">
         <v>176</v>
       </c>
       <c r="I30" s="2">
@@ -1544,7 +1618,7 @@
         <v>85</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="M30" s="2">
         <v>77</v>
@@ -1557,10 +1631,14 @@
       <c r="B31" s="2">
         <v>78</v>
       </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9">
+      <c r="D31" s="7">
+        <v>11.12</v>
+      </c>
+      <c r="E31" s="7">
+        <v>11.15</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7">
         <v>177</v>
       </c>
       <c r="I31" s="2">
@@ -1583,10 +1661,14 @@
       <c r="B32" s="2">
         <v>79</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9">
+      <c r="D32" s="7">
+        <v>11.08</v>
+      </c>
+      <c r="E32" s="7">
+        <v>11.11</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7">
         <v>178</v>
       </c>
       <c r="I32" s="2">
@@ -1609,10 +1691,14 @@
       <c r="B33" s="2">
         <v>80</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9">
+      <c r="D33" s="7">
+        <v>11.04</v>
+      </c>
+      <c r="E33" s="7">
+        <v>11.07</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7">
         <v>179</v>
       </c>
       <c r="I33" s="2">
@@ -1635,10 +1721,14 @@
       <c r="B34" s="2">
         <v>81</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9">
+      <c r="D34" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="7">
+        <v>11.03</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7">
         <v>180</v>
       </c>
       <c r="I34" s="2">
@@ -1661,10 +1751,14 @@
       <c r="B35" s="2">
         <v>82</v>
       </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9">
+      <c r="D35" s="7">
+        <v>10.96</v>
+      </c>
+      <c r="E35" s="7">
+        <v>10.99</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7">
         <v>181</v>
       </c>
       <c r="I35" s="2">
@@ -1687,10 +1781,14 @@
       <c r="B36" s="2">
         <v>83</v>
       </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9">
+      <c r="D36" s="7">
+        <v>10.92</v>
+      </c>
+      <c r="E36" s="7">
+        <v>10.95</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7">
         <v>182</v>
       </c>
       <c r="I36" s="2">
@@ -1713,10 +1811,14 @@
       <c r="B37" s="2">
         <v>84</v>
       </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9">
+      <c r="D37" s="7">
+        <v>10.88</v>
+      </c>
+      <c r="E37" s="7">
+        <v>10.91</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7">
         <v>183</v>
       </c>
       <c r="I37" s="2">
@@ -1739,10 +1841,14 @@
       <c r="B38" s="2">
         <v>85</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9">
+      <c r="D38" s="7">
+        <v>10.84</v>
+      </c>
+      <c r="E38" s="7">
+        <v>10.87</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7">
         <v>184</v>
       </c>
       <c r="I38" s="2">
@@ -1765,10 +1871,14 @@
       <c r="B39" s="2">
         <v>86</v>
       </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9">
+      <c r="D39" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" s="7">
+        <v>10.83</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7">
         <v>185</v>
       </c>
       <c r="I39" s="2">
@@ -1791,10 +1901,14 @@
       <c r="B40" s="2">
         <v>87</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9">
+      <c r="D40" s="7">
+        <v>10.76</v>
+      </c>
+      <c r="E40" s="7">
+        <v>10.79</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7">
         <v>186</v>
       </c>
       <c r="I40" s="2">
@@ -1817,10 +1931,14 @@
       <c r="B41" s="2">
         <v>88</v>
       </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9">
+      <c r="D41" s="7">
+        <v>10.72</v>
+      </c>
+      <c r="E41" s="7">
+        <v>10.75</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7">
         <v>187</v>
       </c>
       <c r="I41" s="2">
@@ -1843,10 +1961,14 @@
       <c r="B42" s="2">
         <v>89</v>
       </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9">
+      <c r="D42" s="7">
+        <v>10.68</v>
+      </c>
+      <c r="E42" s="7">
+        <v>10.71</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7">
         <v>188</v>
       </c>
       <c r="I42" s="2">
@@ -1869,10 +1991,14 @@
       <c r="B43" s="2">
         <v>90</v>
       </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9">
+      <c r="D43" s="7">
+        <v>10.64</v>
+      </c>
+      <c r="E43" s="7">
+        <v>10.67</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7">
         <v>189</v>
       </c>
       <c r="I43" s="2">
@@ -1895,10 +2021,14 @@
       <c r="B44" s="2">
         <v>91</v>
       </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9">
+      <c r="D44" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E44" s="7">
+        <v>10.63</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7">
         <v>190</v>
       </c>
       <c r="I44" s="2" t="s">
@@ -1921,10 +2051,14 @@
       <c r="B45" s="2">
         <v>92</v>
       </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9">
+      <c r="D45" s="7">
+        <v>10.56</v>
+      </c>
+      <c r="E45" s="7">
+        <v>10.59</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7">
         <v>191</v>
       </c>
       <c r="L45" s="2" t="s">
@@ -1941,10 +2075,14 @@
       <c r="B46" s="2">
         <v>93</v>
       </c>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9">
+      <c r="D46" s="7">
+        <v>10.52</v>
+      </c>
+      <c r="E46" s="7">
+        <v>10.55</v>
+      </c>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7">
         <v>192</v>
       </c>
       <c r="L46" s="2" t="s">
@@ -1961,10 +2099,14 @@
       <c r="B47" s="2">
         <v>94</v>
       </c>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9">
+      <c r="D47" s="7">
+        <v>10.48</v>
+      </c>
+      <c r="E47" s="7">
+        <v>10.51</v>
+      </c>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7">
         <v>193</v>
       </c>
       <c r="L47" s="2" t="s">
@@ -1981,10 +2123,14 @@
       <c r="B48" s="2">
         <v>95</v>
       </c>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9">
+      <c r="D48" s="7">
+        <v>10.44</v>
+      </c>
+      <c r="E48" s="7">
+        <v>10.47</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7">
         <v>194</v>
       </c>
       <c r="L48" s="2" t="s">
@@ -2001,10 +2147,14 @@
       <c r="B49" s="2">
         <v>96</v>
       </c>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9">
+      <c r="D49" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E49" s="7">
+        <v>10.43</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7">
         <v>195</v>
       </c>
       <c r="L49" s="2" t="s">
@@ -2021,10 +2171,14 @@
       <c r="B50" s="2">
         <v>97</v>
       </c>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9">
+      <c r="D50" s="7">
+        <v>10.36</v>
+      </c>
+      <c r="E50" s="7">
+        <v>10.39</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7">
         <v>196</v>
       </c>
       <c r="L50" s="2" t="s">
@@ -2041,10 +2195,14 @@
       <c r="B51" s="2">
         <v>98</v>
       </c>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9">
+      <c r="D51" s="7">
+        <v>10.32</v>
+      </c>
+      <c r="E51" s="7">
+        <v>10.35</v>
+      </c>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7">
         <v>197</v>
       </c>
       <c r="L51" s="2" t="s">
@@ -2061,10 +2219,14 @@
       <c r="B52" s="2">
         <v>99</v>
       </c>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9">
+      <c r="D52" s="7">
+        <v>10.28</v>
+      </c>
+      <c r="E52" s="7">
+        <v>10.31</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7">
         <v>198</v>
       </c>
       <c r="L52" s="2" t="s">
@@ -2079,14 +2241,14 @@
     <sortCondition ref="D3:D27"/>
   </sortState>
   <mergeCells count="8">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="D1:G1"/>
     <mergeCell ref="D8:G11"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="D5:G7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="D1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>